<commit_message>
Give dashboard summary for Kepala Penjamin Kualitas Data
</commit_message>
<xml_diff>
--- a/public/template import/Format Import SP2DK.xlsx
+++ b/public/template import/Format Import SP2DK.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam Yordan\Desktop\Surat\template import\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project_Belajar\sp2dk\public\template import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD3827D9-E51E-4DB4-B914-A2D319139E3A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9267625-D157-4CE5-9220-BE9C9D5EEC2E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="15375" windowHeight="8325" xr2:uid="{626D9CD8-A68D-4FAD-97C1-C192B740F3F9}"/>
+    <workbookView xWindow="5115" yWindow="3195" windowWidth="15375" windowHeight="8325" xr2:uid="{626D9CD8-A68D-4FAD-97C1-C192B740F3F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,12 +30,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>NPWP</t>
-  </si>
-  <si>
-    <t>Nama</t>
   </si>
   <si>
     <t>Nomor_SP2DK</t>
@@ -56,7 +53,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -106,7 +103,7 @@
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -422,20 +419,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6A8B0C6-6880-4992-B07F-28D5C91FE5C3}">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -448,11 +445,8 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>